<commit_message>
new instances with 10 and 20 vars
</commit_message>
<xml_diff>
--- a/data/EasternMassachusetts/EM_creation.xlsx
+++ b/data/EasternMassachusetts/EM_creation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/NetbeansProjects/DNDP/data/EasternMassachusetts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Documents/NetbeansProjects/CNDP/data/EasternMassachusetts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6EB3A4-6EDD-3948-BBB9-FE3770E4705B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF1F766-5878-C54F-B1D3-09FACE283C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{3C18C25E-1802-D24A-AE80-06DE8A175B15}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -496,7 +496,7 @@
   <dimension ref="A1:S257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection sqref="A1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -607,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <f ca="1">IF(COUNTIF(N$10:N$19, S10)&gt;0, RAND()*0.02, 0)</f>
+        <f ca="1">IF(COUNTIF(N$10:N$29, S10)&gt;0, RAND()*0.02, 0)</f>
         <v>0</v>
       </c>
       <c r="N10">
@@ -618,7 +618,7 @@
       </c>
       <c r="S10" s="1" cm="1">
         <f t="array" aca="1" ref="S10:S257" ca="1">_xlfn.SORTBY(_xlfn.SEQUENCE(248), _xlfn.RANDARRAY(248))</f>
-        <v>148</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -653,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="K11:K74" ca="1" si="0">IF(COUNTIF(N$10:N$19, S11)&gt;0, RAND()*0.02, 0)</f>
+        <f t="shared" ref="K11:K74" ca="1" si="0">IF(COUNTIF(N$10:N$29, S11)&gt;0, RAND()*0.02, 0)</f>
         <v>0</v>
       </c>
       <c r="N11">
@@ -666,7 +666,7 @@
       </c>
       <c r="S11">
         <f ca="1"/>
-        <v>207</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -714,7 +714,7 @@
       </c>
       <c r="S12">
         <f ca="1"/>
-        <v>189</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
@@ -762,7 +762,7 @@
       </c>
       <c r="S13">
         <f ca="1"/>
-        <v>225</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(COUNTIF(N$10:N$29, S14)&gt;0, RAND()*0.02, 0)</f>
         <v>0</v>
       </c>
       <c r="N14">
@@ -810,7 +810,7 @@
       </c>
       <c r="S14">
         <f ca="1"/>
-        <v>235</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -858,7 +858,7 @@
       </c>
       <c r="S15">
         <f ca="1"/>
-        <v>93</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -906,7 +906,7 @@
       </c>
       <c r="S16">
         <f ca="1"/>
-        <v>68</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
@@ -941,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(COUNTIF(N$10:N$29, S17)&gt;0, RAND()*0.02, 0)</f>
         <v>0</v>
       </c>
       <c r="N17">
@@ -954,7 +954,7 @@
       </c>
       <c r="S17">
         <f ca="1"/>
-        <v>37</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
@@ -1002,7 +1002,7 @@
       </c>
       <c r="S18">
         <f ca="1"/>
-        <v>134</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
@@ -1050,7 +1050,7 @@
       </c>
       <c r="S19">
         <f ca="1"/>
-        <v>149</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="S20">
         <f ca="1"/>
-        <v>94</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
@@ -1146,7 +1146,7 @@
       </c>
       <c r="S21">
         <f ca="1"/>
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="S22">
         <f ca="1"/>
-        <v>234</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
@@ -1242,7 +1242,7 @@
       </c>
       <c r="S23">
         <f ca="1"/>
-        <v>117</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="S24">
         <f ca="1"/>
-        <v>45</v>
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="S25">
         <f ca="1"/>
-        <v>203</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
@@ -1386,7 +1386,7 @@
       </c>
       <c r="S26">
         <f ca="1"/>
-        <v>21</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
@@ -1434,7 +1434,7 @@
       </c>
       <c r="S27">
         <f ca="1"/>
-        <v>196</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="S28">
         <f ca="1"/>
-        <v>60</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="S29">
         <f ca="1"/>
-        <v>204</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
@@ -1578,7 +1578,7 @@
       </c>
       <c r="S30">
         <f ca="1"/>
-        <v>192</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="S31">
         <f ca="1"/>
-        <v>172</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
@@ -1674,7 +1674,7 @@
       </c>
       <c r="S32">
         <f ca="1"/>
-        <v>124</v>
+        <v>147</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
@@ -1722,7 +1722,7 @@
       </c>
       <c r="S33">
         <f ca="1"/>
-        <v>78</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="S34">
         <f ca="1"/>
-        <v>15</v>
+        <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="S35">
         <f ca="1"/>
-        <v>159</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="S36">
         <f ca="1"/>
-        <v>54</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="S37">
         <f ca="1"/>
-        <v>230</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="S38">
         <f ca="1"/>
-        <v>211</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="S39">
         <f ca="1"/>
-        <v>147</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
@@ -2054,7 +2054,7 @@
       </c>
       <c r="S40">
         <f ca="1"/>
-        <v>150</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="S41">
         <f ca="1"/>
-        <v>89</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="S42">
         <f ca="1"/>
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
@@ -2186,7 +2186,7 @@
       </c>
       <c r="S43">
         <f ca="1"/>
-        <v>200</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="S44">
         <f ca="1"/>
-        <v>220</v>
+        <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="S45">
         <f ca="1"/>
-        <v>190</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
@@ -2318,7 +2318,7 @@
       </c>
       <c r="S46">
         <f ca="1"/>
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="K47">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2.9546209891908215E-3</v>
       </c>
       <c r="N47">
         <f t="shared" si="1"/>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="S47">
         <f ca="1"/>
-        <v>40</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
@@ -2406,7 +2406,7 @@
       </c>
       <c r="S48">
         <f ca="1"/>
-        <v>99</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.2">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="S49">
         <f ca="1"/>
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="S50">
         <f ca="1"/>
-        <v>212</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.2">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="S51">
         <f ca="1"/>
-        <v>114</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.2">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="S52">
         <f ca="1"/>
-        <v>168</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.2">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="S53">
         <f ca="1"/>
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
@@ -2670,7 +2670,7 @@
       </c>
       <c r="S54">
         <f ca="1"/>
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.2">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="K55">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>8.8819261532377212E-3</v>
       </c>
       <c r="N55">
         <f t="shared" si="1"/>
@@ -2714,7 +2714,7 @@
       </c>
       <c r="S55">
         <f ca="1"/>
-        <v>191</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.2">
@@ -2758,7 +2758,7 @@
       </c>
       <c r="S56">
         <f ca="1"/>
-        <v>210</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.2">
@@ -2802,7 +2802,7 @@
       </c>
       <c r="S57">
         <f ca="1"/>
-        <v>184</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.2">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="S58">
         <f ca="1"/>
-        <v>199</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.2">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="S59">
         <f ca="1"/>
-        <v>157</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
@@ -2926,7 +2926,7 @@
       </c>
       <c r="K60">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4506016059050382E-3</v>
+        <v>0</v>
       </c>
       <c r="N60">
         <f t="shared" si="1"/>
@@ -2934,7 +2934,7 @@
       </c>
       <c r="S60">
         <f ca="1"/>
-        <v>3</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="K61">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1.5647512737254617E-2</v>
       </c>
       <c r="N61">
         <f t="shared" si="1"/>
@@ -2978,7 +2978,7 @@
       </c>
       <c r="S61">
         <f ca="1"/>
-        <v>105</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
@@ -3022,7 +3022,7 @@
       </c>
       <c r="S62">
         <f ca="1"/>
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.2">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="S63">
         <f ca="1"/>
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.2">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="S64">
         <f ca="1"/>
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.2">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="K65">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1.1689172841300468E-2</v>
       </c>
       <c r="N65">
         <f t="shared" si="1"/>
@@ -3154,7 +3154,7 @@
       </c>
       <c r="S65">
         <f ca="1"/>
-        <v>107</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
@@ -3198,7 +3198,7 @@
       </c>
       <c r="S66">
         <f ca="1"/>
-        <v>91</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.2">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="S67">
         <f ca="1"/>
-        <v>43</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.2">
@@ -3286,7 +3286,7 @@
       </c>
       <c r="S68">
         <f ca="1"/>
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.2">
@@ -3330,7 +3330,7 @@
       </c>
       <c r="S69">
         <f ca="1"/>
-        <v>165</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.2">
@@ -3374,7 +3374,7 @@
       </c>
       <c r="S70">
         <f ca="1"/>
-        <v>36</v>
+        <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.2">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="S71">
         <f ca="1"/>
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.2">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="S72">
         <f ca="1"/>
-        <v>208</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.2">
@@ -3498,7 +3498,7 @@
       </c>
       <c r="K73">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1.8512711019838327E-2</v>
       </c>
       <c r="N73">
         <f t="shared" si="1"/>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="S73">
         <f ca="1"/>
-        <v>56</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.2">
@@ -3550,7 +3550,7 @@
       </c>
       <c r="S74">
         <f ca="1"/>
-        <v>82</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.2">
@@ -3585,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="K75">
-        <f t="shared" ref="K75:K138" ca="1" si="3">IF(COUNTIF(N$10:N$19, S75)&gt;0, RAND()*0.02, 0)</f>
+        <f t="shared" ref="K75:K138" ca="1" si="3">IF(COUNTIF(N$10:N$29, S75)&gt;0, RAND()*0.02, 0)</f>
         <v>0</v>
       </c>
       <c r="N75">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="S75">
         <f ca="1"/>
-        <v>139</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.2">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="S76">
         <f ca="1"/>
-        <v>110</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.2">
@@ -3682,7 +3682,7 @@
       </c>
       <c r="S77">
         <f ca="1"/>
-        <v>27</v>
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.2">
@@ -3726,7 +3726,7 @@
       </c>
       <c r="S78">
         <f ca="1"/>
-        <v>70</v>
+        <v>115</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.2">
@@ -3770,7 +3770,7 @@
       </c>
       <c r="S79">
         <f ca="1"/>
-        <v>126</v>
+        <v>21</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.2">
@@ -3814,7 +3814,7 @@
       </c>
       <c r="S80">
         <f ca="1"/>
-        <v>164</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.2">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="S81">
         <f ca="1"/>
-        <v>83</v>
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.2">
@@ -3894,7 +3894,7 @@
       </c>
       <c r="K82">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>7.3872501996032148E-3</v>
       </c>
       <c r="N82">
         <f t="shared" si="4"/>
@@ -3902,7 +3902,7 @@
       </c>
       <c r="S82">
         <f ca="1"/>
-        <v>240</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.2">
@@ -3938,7 +3938,7 @@
       </c>
       <c r="K83">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>2.7417831482437374E-4</v>
       </c>
       <c r="N83">
         <f t="shared" si="4"/>
@@ -3946,7 +3946,7 @@
       </c>
       <c r="S83">
         <f ca="1"/>
-        <v>182</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.2">
@@ -3982,7 +3982,7 @@
       </c>
       <c r="K84">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>8.3644046954742366E-4</v>
       </c>
       <c r="N84">
         <f t="shared" si="4"/>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="S84">
         <f ca="1"/>
-        <v>158</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.2">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="S85">
         <f ca="1"/>
-        <v>130</v>
+        <v>74</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.2">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="S86">
         <f ca="1"/>
-        <v>227</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.2">
@@ -4122,7 +4122,7 @@
       </c>
       <c r="S87">
         <f ca="1"/>
-        <v>127</v>
+        <v>48</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.2">
@@ -4166,7 +4166,7 @@
       </c>
       <c r="S88">
         <f ca="1"/>
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.2">
@@ -4210,7 +4210,7 @@
       </c>
       <c r="S89">
         <f ca="1"/>
-        <v>224</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.2">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="S90">
         <f ca="1"/>
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.2">
@@ -4298,7 +4298,7 @@
       </c>
       <c r="S91">
         <f ca="1"/>
-        <v>153</v>
+        <v>125</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.2">
@@ -4342,7 +4342,7 @@
       </c>
       <c r="S92">
         <f ca="1"/>
-        <v>193</v>
+        <v>240</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.2">
@@ -4378,7 +4378,7 @@
       </c>
       <c r="K93">
         <f t="shared" ca="1" si="3"/>
-        <v>1.4174885016769063E-2</v>
+        <v>0</v>
       </c>
       <c r="N93">
         <f t="shared" si="4"/>
@@ -4386,7 +4386,7 @@
       </c>
       <c r="S93">
         <f ca="1"/>
-        <v>7</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.2">
@@ -4430,7 +4430,7 @@
       </c>
       <c r="S94">
         <f ca="1"/>
-        <v>11</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.2">
@@ -4474,7 +4474,7 @@
       </c>
       <c r="S95">
         <f ca="1"/>
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.2">
@@ -4518,7 +4518,7 @@
       </c>
       <c r="S96">
         <f ca="1"/>
-        <v>46</v>
+        <v>200</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.2">
@@ -4562,7 +4562,7 @@
       </c>
       <c r="S97">
         <f ca="1"/>
-        <v>247</v>
+        <v>60</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.2">
@@ -4606,7 +4606,7 @@
       </c>
       <c r="S98">
         <f ca="1"/>
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.2">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="S99">
         <f ca="1"/>
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.2">
@@ -4694,7 +4694,7 @@
       </c>
       <c r="S100">
         <f ca="1"/>
-        <v>92</v>
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.2">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="K101">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>8.4670430700302633E-3</v>
       </c>
       <c r="N101">
         <f t="shared" si="4"/>
@@ -4738,7 +4738,7 @@
       </c>
       <c r="S101">
         <f ca="1"/>
-        <v>31</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.2">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="S102">
         <f ca="1"/>
-        <v>232</v>
+        <v>160</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.2">
@@ -4826,7 +4826,7 @@
       </c>
       <c r="S103">
         <f ca="1"/>
-        <v>188</v>
+        <v>248</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.2">
@@ -4870,7 +4870,7 @@
       </c>
       <c r="S104">
         <f ca="1"/>
-        <v>22</v>
+        <v>218</v>
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.2">
@@ -4914,7 +4914,7 @@
       </c>
       <c r="S105">
         <f ca="1"/>
-        <v>58</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.2">
@@ -4958,7 +4958,7 @@
       </c>
       <c r="S106">
         <f ca="1"/>
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.2">
@@ -5002,7 +5002,7 @@
       </c>
       <c r="S107">
         <f ca="1"/>
-        <v>166</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.2">
@@ -5038,7 +5038,7 @@
       </c>
       <c r="K108">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>6.9238716272738187E-3</v>
       </c>
       <c r="N108">
         <f t="shared" si="4"/>
@@ -5046,7 +5046,7 @@
       </c>
       <c r="S108">
         <f ca="1"/>
-        <v>219</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.2">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="K109">
         <f t="shared" ca="1" si="3"/>
-        <v>3.7890214579648228E-3</v>
+        <v>0</v>
       </c>
       <c r="N109">
         <f t="shared" si="4"/>
@@ -5090,7 +5090,7 @@
       </c>
       <c r="S109">
         <f ca="1"/>
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.2">
@@ -5134,7 +5134,7 @@
       </c>
       <c r="S110">
         <f ca="1"/>
-        <v>29</v>
+        <v>224</v>
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.2">
@@ -5178,7 +5178,7 @@
       </c>
       <c r="S111">
         <f ca="1"/>
-        <v>162</v>
+        <v>91</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.2">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="S112">
         <f ca="1"/>
-        <v>59</v>
+        <v>145</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.2">
@@ -5266,7 +5266,7 @@
       </c>
       <c r="S113">
         <f ca="1"/>
-        <v>44</v>
+        <v>236</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.2">
@@ -5310,7 +5310,7 @@
       </c>
       <c r="S114">
         <f ca="1"/>
-        <v>32</v>
+        <v>189</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.2">
@@ -5354,7 +5354,7 @@
       </c>
       <c r="S115">
         <f ca="1"/>
-        <v>19</v>
+        <v>241</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.2">
@@ -5390,7 +5390,7 @@
       </c>
       <c r="K116">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1.3739150841011603E-2</v>
       </c>
       <c r="N116">
         <f t="shared" si="4"/>
@@ -5398,7 +5398,7 @@
       </c>
       <c r="S116">
         <f ca="1"/>
-        <v>175</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.2">
@@ -5442,7 +5442,7 @@
       </c>
       <c r="S117">
         <f ca="1"/>
-        <v>109</v>
+        <v>177</v>
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.2">
@@ -5486,7 +5486,7 @@
       </c>
       <c r="S118">
         <f ca="1"/>
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.2">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="S119">
         <f ca="1"/>
-        <v>201</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.2">
@@ -5574,7 +5574,7 @@
       </c>
       <c r="S120">
         <f ca="1"/>
-        <v>195</v>
+        <v>82</v>
       </c>
     </row>
     <row r="121" spans="1:19" x14ac:dyDescent="0.2">
@@ -5618,7 +5618,7 @@
       </c>
       <c r="S121">
         <f ca="1"/>
-        <v>229</v>
+        <v>107</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.2">
@@ -5662,7 +5662,7 @@
       </c>
       <c r="S122">
         <f ca="1"/>
-        <v>151</v>
+        <v>167</v>
       </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.2">
@@ -5706,7 +5706,7 @@
       </c>
       <c r="S123">
         <f ca="1"/>
-        <v>213</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.2">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="S124">
         <f ca="1"/>
-        <v>163</v>
+        <v>237</v>
       </c>
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.2">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="S125">
         <f ca="1"/>
-        <v>129</v>
+        <v>98</v>
       </c>
     </row>
     <row r="126" spans="1:19" x14ac:dyDescent="0.2">
@@ -5838,7 +5838,7 @@
       </c>
       <c r="S126">
         <f ca="1"/>
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="127" spans="1:19" x14ac:dyDescent="0.2">
@@ -5882,7 +5882,7 @@
       </c>
       <c r="S127">
         <f ca="1"/>
-        <v>101</v>
+        <v>148</v>
       </c>
     </row>
     <row r="128" spans="1:19" x14ac:dyDescent="0.2">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="K128">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3.5782665385030257E-3</v>
       </c>
       <c r="N128">
         <f t="shared" si="4"/>
@@ -5926,7 +5926,7 @@
       </c>
       <c r="S128">
         <f ca="1"/>
-        <v>226</v>
+        <v>16</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.2">
@@ -5962,7 +5962,7 @@
       </c>
       <c r="K129">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3.0489209560582474E-3</v>
       </c>
       <c r="N129">
         <f t="shared" si="4"/>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="S129">
         <f ca="1"/>
-        <v>65</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.2">
@@ -6014,7 +6014,7 @@
       </c>
       <c r="S130">
         <f ca="1"/>
-        <v>132</v>
+        <v>182</v>
       </c>
     </row>
     <row r="131" spans="1:19" x14ac:dyDescent="0.2">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="K131">
         <f t="shared" ca="1" si="3"/>
-        <v>8.223333308297465E-3</v>
+        <v>0</v>
       </c>
       <c r="N131">
         <f t="shared" si="4"/>
@@ -6058,7 +6058,7 @@
       </c>
       <c r="S131">
         <f ca="1"/>
-        <v>1</v>
+        <v>73</v>
       </c>
     </row>
     <row r="132" spans="1:19" x14ac:dyDescent="0.2">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="S132">
         <f ca="1"/>
-        <v>198</v>
+        <v>151</v>
       </c>
     </row>
     <row r="133" spans="1:19" x14ac:dyDescent="0.2">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="S133">
         <f ca="1"/>
-        <v>170</v>
+        <v>58</v>
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.2">
@@ -6190,7 +6190,7 @@
       </c>
       <c r="S134">
         <f ca="1"/>
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.2">
@@ -6234,7 +6234,7 @@
       </c>
       <c r="S135">
         <f ca="1"/>
-        <v>63</v>
+        <v>103</v>
       </c>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.2">
@@ -6278,7 +6278,7 @@
       </c>
       <c r="S136">
         <f ca="1"/>
-        <v>156</v>
+        <v>81</v>
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.2">
@@ -6322,7 +6322,7 @@
       </c>
       <c r="S137">
         <f ca="1"/>
-        <v>140</v>
+        <v>217</v>
       </c>
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.2">
@@ -6366,7 +6366,7 @@
       </c>
       <c r="S138">
         <f ca="1"/>
-        <v>47</v>
+        <v>140</v>
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.2">
@@ -6401,7 +6401,7 @@
         <v>0</v>
       </c>
       <c r="K139">
-        <f t="shared" ref="K139:K202" ca="1" si="5">IF(COUNTIF(N$10:N$19, S139)&gt;0, RAND()*0.02, 0)</f>
+        <f t="shared" ref="K139:K202" ca="1" si="5">IF(COUNTIF(N$10:N$29, S139)&gt;0, RAND()*0.02, 0)</f>
         <v>0</v>
       </c>
       <c r="N139">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="S139">
         <f ca="1"/>
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.2">
@@ -6446,7 +6446,7 @@
       </c>
       <c r="K140">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>7.7561010473166259E-3</v>
       </c>
       <c r="N140">
         <f t="shared" ref="N140:N203" si="6">N139+1</f>
@@ -6454,7 +6454,7 @@
       </c>
       <c r="S140">
         <f ca="1"/>
-        <v>155</v>
+        <v>15</v>
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.2">
@@ -6498,7 +6498,7 @@
       </c>
       <c r="S141">
         <f ca="1"/>
-        <v>185</v>
+        <v>144</v>
       </c>
     </row>
     <row r="142" spans="1:19" x14ac:dyDescent="0.2">
@@ -6534,7 +6534,7 @@
       </c>
       <c r="K142">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1.1276938126190501E-2</v>
       </c>
       <c r="N142">
         <f t="shared" si="6"/>
@@ -6542,7 +6542,7 @@
       </c>
       <c r="S142">
         <f ca="1"/>
-        <v>39</v>
+        <v>19</v>
       </c>
     </row>
     <row r="143" spans="1:19" x14ac:dyDescent="0.2">
@@ -6586,7 +6586,7 @@
       </c>
       <c r="S143">
         <f ca="1"/>
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.2">
@@ -6630,7 +6630,7 @@
       </c>
       <c r="S144">
         <f ca="1"/>
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="145" spans="1:19" x14ac:dyDescent="0.2">
@@ -6674,7 +6674,7 @@
       </c>
       <c r="S145">
         <f ca="1"/>
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="146" spans="1:19" x14ac:dyDescent="0.2">
@@ -6718,7 +6718,7 @@
       </c>
       <c r="S146">
         <f ca="1"/>
-        <v>16</v>
+        <v>95</v>
       </c>
     </row>
     <row r="147" spans="1:19" x14ac:dyDescent="0.2">
@@ -6762,7 +6762,7 @@
       </c>
       <c r="S147">
         <f ca="1"/>
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="148" spans="1:19" x14ac:dyDescent="0.2">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="S148">
         <f ca="1"/>
-        <v>116</v>
+        <v>199</v>
       </c>
     </row>
     <row r="149" spans="1:19" x14ac:dyDescent="0.2">
@@ -6850,7 +6850,7 @@
       </c>
       <c r="S149">
         <f ca="1"/>
-        <v>51</v>
+        <v>159</v>
       </c>
     </row>
     <row r="150" spans="1:19" x14ac:dyDescent="0.2">
@@ -6894,7 +6894,7 @@
       </c>
       <c r="S150">
         <f ca="1"/>
-        <v>111</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151" spans="1:19" x14ac:dyDescent="0.2">
@@ -6938,7 +6938,7 @@
       </c>
       <c r="S151">
         <f ca="1"/>
-        <v>137</v>
+        <v>44</v>
       </c>
     </row>
     <row r="152" spans="1:19" x14ac:dyDescent="0.2">
@@ -6982,7 +6982,7 @@
       </c>
       <c r="S152">
         <f ca="1"/>
-        <v>160</v>
+        <v>68</v>
       </c>
     </row>
     <row r="153" spans="1:19" x14ac:dyDescent="0.2">
@@ -7026,7 +7026,7 @@
       </c>
       <c r="S153">
         <f ca="1"/>
-        <v>154</v>
+        <v>230</v>
       </c>
     </row>
     <row r="154" spans="1:19" x14ac:dyDescent="0.2">
@@ -7070,7 +7070,7 @@
       </c>
       <c r="S154">
         <f ca="1"/>
-        <v>34</v>
+        <v>220</v>
       </c>
     </row>
     <row r="155" spans="1:19" x14ac:dyDescent="0.2">
@@ -7114,7 +7114,7 @@
       </c>
       <c r="S155">
         <f ca="1"/>
-        <v>179</v>
+        <v>227</v>
       </c>
     </row>
     <row r="156" spans="1:19" x14ac:dyDescent="0.2">
@@ -7158,7 +7158,7 @@
       </c>
       <c r="S156">
         <f ca="1"/>
-        <v>41</v>
+        <v>134</v>
       </c>
     </row>
     <row r="157" spans="1:19" x14ac:dyDescent="0.2">
@@ -7202,7 +7202,7 @@
       </c>
       <c r="S157">
         <f ca="1"/>
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="158" spans="1:19" x14ac:dyDescent="0.2">
@@ -7246,7 +7246,7 @@
       </c>
       <c r="S158">
         <f ca="1"/>
-        <v>102</v>
+        <v>202</v>
       </c>
     </row>
     <row r="159" spans="1:19" x14ac:dyDescent="0.2">
@@ -7290,7 +7290,7 @@
       </c>
       <c r="S159">
         <f ca="1"/>
-        <v>144</v>
+        <v>88</v>
       </c>
     </row>
     <row r="160" spans="1:19" x14ac:dyDescent="0.2">
@@ -7334,7 +7334,7 @@
       </c>
       <c r="S160">
         <f ca="1"/>
-        <v>222</v>
+        <v>100</v>
       </c>
     </row>
     <row r="161" spans="1:19" x14ac:dyDescent="0.2">
@@ -7378,7 +7378,7 @@
       </c>
       <c r="S161">
         <f ca="1"/>
-        <v>96</v>
+        <v>168</v>
       </c>
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.2">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="S162">
         <f ca="1"/>
-        <v>135</v>
+        <v>174</v>
       </c>
     </row>
     <row r="163" spans="1:19" x14ac:dyDescent="0.2">
@@ -7466,7 +7466,7 @@
       </c>
       <c r="S163">
         <f ca="1"/>
-        <v>120</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:19" x14ac:dyDescent="0.2">
@@ -7510,7 +7510,7 @@
       </c>
       <c r="S164">
         <f ca="1"/>
-        <v>174</v>
+        <v>23</v>
       </c>
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.2">
@@ -7554,7 +7554,7 @@
       </c>
       <c r="S165">
         <f ca="1"/>
-        <v>128</v>
+        <v>164</v>
       </c>
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.2">
@@ -7598,7 +7598,7 @@
       </c>
       <c r="S166">
         <f ca="1"/>
-        <v>142</v>
+        <v>212</v>
       </c>
     </row>
     <row r="167" spans="1:19" x14ac:dyDescent="0.2">
@@ -7642,7 +7642,7 @@
       </c>
       <c r="S167">
         <f ca="1"/>
-        <v>173</v>
+        <v>85</v>
       </c>
     </row>
     <row r="168" spans="1:19" x14ac:dyDescent="0.2">
@@ -7678,7 +7678,7 @@
       </c>
       <c r="K168">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>1.3360357552294033E-3</v>
       </c>
       <c r="N168">
         <f t="shared" si="6"/>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="S168">
         <f ca="1"/>
-        <v>79</v>
+        <v>13</v>
       </c>
     </row>
     <row r="169" spans="1:19" x14ac:dyDescent="0.2">
@@ -7730,7 +7730,7 @@
       </c>
       <c r="S169">
         <f ca="1"/>
-        <v>49</v>
+        <v>141</v>
       </c>
     </row>
     <row r="170" spans="1:19" x14ac:dyDescent="0.2">
@@ -7774,7 +7774,7 @@
       </c>
       <c r="S170">
         <f ca="1"/>
-        <v>141</v>
+        <v>64</v>
       </c>
     </row>
     <row r="171" spans="1:19" x14ac:dyDescent="0.2">
@@ -7818,7 +7818,7 @@
       </c>
       <c r="S171">
         <f ca="1"/>
-        <v>121</v>
+        <v>206</v>
       </c>
     </row>
     <row r="172" spans="1:19" x14ac:dyDescent="0.2">
@@ -7862,7 +7862,7 @@
       </c>
       <c r="S172">
         <f ca="1"/>
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="173" spans="1:19" x14ac:dyDescent="0.2">
@@ -7906,7 +7906,7 @@
       </c>
       <c r="S173">
         <f ca="1"/>
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="174" spans="1:19" x14ac:dyDescent="0.2">
@@ -7950,7 +7950,7 @@
       </c>
       <c r="S174">
         <f ca="1"/>
-        <v>85</v>
+        <v>122</v>
       </c>
     </row>
     <row r="175" spans="1:19" x14ac:dyDescent="0.2">
@@ -7994,7 +7994,7 @@
       </c>
       <c r="S175">
         <f ca="1"/>
-        <v>73</v>
+        <v>172</v>
       </c>
     </row>
     <row r="176" spans="1:19" x14ac:dyDescent="0.2">
@@ -8038,7 +8038,7 @@
       </c>
       <c r="S176">
         <f ca="1"/>
-        <v>202</v>
+        <v>176</v>
       </c>
     </row>
     <row r="177" spans="1:19" x14ac:dyDescent="0.2">
@@ -8082,7 +8082,7 @@
       </c>
       <c r="S177">
         <f ca="1"/>
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="178" spans="1:19" x14ac:dyDescent="0.2">
@@ -8126,7 +8126,7 @@
       </c>
       <c r="S178">
         <f ca="1"/>
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="179" spans="1:19" x14ac:dyDescent="0.2">
@@ -8170,7 +8170,7 @@
       </c>
       <c r="S179">
         <f ca="1"/>
-        <v>35</v>
+        <v>83</v>
       </c>
     </row>
     <row r="180" spans="1:19" x14ac:dyDescent="0.2">
@@ -8206,7 +8206,7 @@
       </c>
       <c r="K180">
         <f t="shared" ca="1" si="5"/>
-        <v>1.1967429728715213E-2</v>
+        <v>0</v>
       </c>
       <c r="N180">
         <f t="shared" si="6"/>
@@ -8214,7 +8214,7 @@
       </c>
       <c r="S180">
         <f ca="1"/>
-        <v>6</v>
+        <v>204</v>
       </c>
     </row>
     <row r="181" spans="1:19" x14ac:dyDescent="0.2">
@@ -8258,7 +8258,7 @@
       </c>
       <c r="S181">
         <f ca="1"/>
-        <v>218</v>
+        <v>71</v>
       </c>
     </row>
     <row r="182" spans="1:19" x14ac:dyDescent="0.2">
@@ -8302,7 +8302,7 @@
       </c>
       <c r="S182">
         <f ca="1"/>
-        <v>23</v>
+        <v>128</v>
       </c>
     </row>
     <row r="183" spans="1:19" x14ac:dyDescent="0.2">
@@ -8346,7 +8346,7 @@
       </c>
       <c r="S183">
         <f ca="1"/>
-        <v>197</v>
+        <v>112</v>
       </c>
     </row>
     <row r="184" spans="1:19" x14ac:dyDescent="0.2">
@@ -8390,7 +8390,7 @@
       </c>
       <c r="S184">
         <f ca="1"/>
-        <v>171</v>
+        <v>152</v>
       </c>
     </row>
     <row r="185" spans="1:19" x14ac:dyDescent="0.2">
@@ -8426,7 +8426,7 @@
       </c>
       <c r="K185">
         <f t="shared" ca="1" si="5"/>
-        <v>5.8244561874457148E-3</v>
+        <v>0</v>
       </c>
       <c r="N185">
         <f t="shared" si="6"/>
@@ -8434,7 +8434,7 @@
       </c>
       <c r="S185">
         <f ca="1"/>
-        <v>8</v>
+        <v>93</v>
       </c>
     </row>
     <row r="186" spans="1:19" x14ac:dyDescent="0.2">
@@ -8478,7 +8478,7 @@
       </c>
       <c r="S186">
         <f ca="1"/>
-        <v>119</v>
+        <v>87</v>
       </c>
     </row>
     <row r="187" spans="1:19" x14ac:dyDescent="0.2">
@@ -8522,7 +8522,7 @@
       </c>
       <c r="S187">
         <f ca="1"/>
-        <v>241</v>
+        <v>196</v>
       </c>
     </row>
     <row r="188" spans="1:19" x14ac:dyDescent="0.2">
@@ -8566,7 +8566,7 @@
       </c>
       <c r="S188">
         <f ca="1"/>
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="189" spans="1:19" x14ac:dyDescent="0.2">
@@ -8610,7 +8610,7 @@
       </c>
       <c r="S189">
         <f ca="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="190" spans="1:19" x14ac:dyDescent="0.2">
@@ -8654,7 +8654,7 @@
       </c>
       <c r="S190">
         <f ca="1"/>
-        <v>95</v>
+        <v>150</v>
       </c>
     </row>
     <row r="191" spans="1:19" x14ac:dyDescent="0.2">
@@ -8698,7 +8698,7 @@
       </c>
       <c r="S191">
         <f ca="1"/>
-        <v>181</v>
+        <v>246</v>
       </c>
     </row>
     <row r="192" spans="1:19" x14ac:dyDescent="0.2">
@@ -8742,7 +8742,7 @@
       </c>
       <c r="S192">
         <f ca="1"/>
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="193" spans="1:19" x14ac:dyDescent="0.2">
@@ -8786,7 +8786,7 @@
       </c>
       <c r="S193">
         <f ca="1"/>
-        <v>123</v>
+        <v>175</v>
       </c>
     </row>
     <row r="194" spans="1:19" x14ac:dyDescent="0.2">
@@ -8830,7 +8830,7 @@
       </c>
       <c r="S194">
         <f ca="1"/>
-        <v>215</v>
+        <v>114</v>
       </c>
     </row>
     <row r="195" spans="1:19" x14ac:dyDescent="0.2">
@@ -8874,7 +8874,7 @@
       </c>
       <c r="S195">
         <f ca="1"/>
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="196" spans="1:19" x14ac:dyDescent="0.2">
@@ -8918,7 +8918,7 @@
       </c>
       <c r="S196">
         <f ca="1"/>
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="197" spans="1:19" x14ac:dyDescent="0.2">
@@ -8962,7 +8962,7 @@
       </c>
       <c r="S197">
         <f ca="1"/>
-        <v>97</v>
+        <v>158</v>
       </c>
     </row>
     <row r="198" spans="1:19" x14ac:dyDescent="0.2">
@@ -9006,7 +9006,7 @@
       </c>
       <c r="S198">
         <f ca="1"/>
-        <v>90</v>
+        <v>42</v>
       </c>
     </row>
     <row r="199" spans="1:19" x14ac:dyDescent="0.2">
@@ -9050,7 +9050,7 @@
       </c>
       <c r="S199">
         <f ca="1"/>
-        <v>104</v>
+        <v>61</v>
       </c>
     </row>
     <row r="200" spans="1:19" x14ac:dyDescent="0.2">
@@ -9094,7 +9094,7 @@
       </c>
       <c r="S200">
         <f ca="1"/>
-        <v>244</v>
+        <v>195</v>
       </c>
     </row>
     <row r="201" spans="1:19" x14ac:dyDescent="0.2">
@@ -9138,7 +9138,7 @@
       </c>
       <c r="S201">
         <f ca="1"/>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="202" spans="1:19" x14ac:dyDescent="0.2">
@@ -9182,7 +9182,7 @@
       </c>
       <c r="S202">
         <f ca="1"/>
-        <v>221</v>
+        <v>27</v>
       </c>
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.2">
@@ -9217,7 +9217,7 @@
         <v>0</v>
       </c>
       <c r="K203">
-        <f t="shared" ref="K203:K257" ca="1" si="7">IF(COUNTIF(N$10:N$19, S203)&gt;0, RAND()*0.02, 0)</f>
+        <f t="shared" ref="K203:K257" ca="1" si="7">IF(COUNTIF(N$10:N$29, S203)&gt;0, RAND()*0.02, 0)</f>
         <v>0</v>
       </c>
       <c r="N203">
@@ -9226,7 +9226,7 @@
       </c>
       <c r="S203">
         <f ca="1"/>
-        <v>238</v>
+        <v>149</v>
       </c>
     </row>
     <row r="204" spans="1:19" x14ac:dyDescent="0.2">
@@ -9270,7 +9270,7 @@
       </c>
       <c r="S204">
         <f ca="1"/>
-        <v>143</v>
+        <v>31</v>
       </c>
     </row>
     <row r="205" spans="1:19" x14ac:dyDescent="0.2">
@@ -9314,7 +9314,7 @@
       </c>
       <c r="S205">
         <f ca="1"/>
-        <v>38</v>
+        <v>180</v>
       </c>
     </row>
     <row r="206" spans="1:19" x14ac:dyDescent="0.2">
@@ -9358,7 +9358,7 @@
       </c>
       <c r="S206">
         <f ca="1"/>
-        <v>194</v>
+        <v>56</v>
       </c>
     </row>
     <row r="207" spans="1:19" x14ac:dyDescent="0.2">
@@ -9402,7 +9402,7 @@
       </c>
       <c r="S207">
         <f ca="1"/>
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.2">
@@ -9446,7 +9446,7 @@
       </c>
       <c r="S208">
         <f ca="1"/>
-        <v>243</v>
+        <v>194</v>
       </c>
     </row>
     <row r="209" spans="1:19" x14ac:dyDescent="0.2">
@@ -9490,7 +9490,7 @@
       </c>
       <c r="S209">
         <f ca="1"/>
-        <v>26</v>
+        <v>47</v>
       </c>
     </row>
     <row r="210" spans="1:19" x14ac:dyDescent="0.2">
@@ -9534,7 +9534,7 @@
       </c>
       <c r="S210">
         <f ca="1"/>
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="211" spans="1:19" x14ac:dyDescent="0.2">
@@ -9578,7 +9578,7 @@
       </c>
       <c r="S211">
         <f ca="1"/>
-        <v>131</v>
+        <v>79</v>
       </c>
     </row>
     <row r="212" spans="1:19" x14ac:dyDescent="0.2">
@@ -9614,7 +9614,7 @@
       </c>
       <c r="K212">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>4.107042012663196E-3</v>
       </c>
       <c r="N212">
         <f t="shared" si="8"/>
@@ -9622,7 +9622,7 @@
       </c>
       <c r="S212">
         <f ca="1"/>
-        <v>183</v>
+        <v>4</v>
       </c>
     </row>
     <row r="213" spans="1:19" x14ac:dyDescent="0.2">
@@ -9666,7 +9666,7 @@
       </c>
       <c r="S213">
         <f ca="1"/>
-        <v>71</v>
+        <v>84</v>
       </c>
     </row>
     <row r="214" spans="1:19" x14ac:dyDescent="0.2">
@@ -9710,7 +9710,7 @@
       </c>
       <c r="S214">
         <f ca="1"/>
-        <v>242</v>
+        <v>53</v>
       </c>
     </row>
     <row r="215" spans="1:19" x14ac:dyDescent="0.2">
@@ -9746,7 +9746,7 @@
       </c>
       <c r="K215">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>2.7772931333241058E-3</v>
       </c>
       <c r="N215">
         <f t="shared" si="8"/>
@@ -9754,7 +9754,7 @@
       </c>
       <c r="S215">
         <f ca="1"/>
-        <v>103</v>
+        <v>12</v>
       </c>
     </row>
     <row r="216" spans="1:19" x14ac:dyDescent="0.2">
@@ -9798,7 +9798,7 @@
       </c>
       <c r="S216">
         <f ca="1"/>
-        <v>28</v>
+        <v>203</v>
       </c>
     </row>
     <row r="217" spans="1:19" x14ac:dyDescent="0.2">
@@ -9834,7 +9834,7 @@
       </c>
       <c r="K217">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>1.2858733025504773E-2</v>
       </c>
       <c r="N217">
         <f t="shared" si="8"/>
@@ -9842,7 +9842,7 @@
       </c>
       <c r="S217">
         <f ca="1"/>
-        <v>248</v>
+        <v>20</v>
       </c>
     </row>
     <row r="218" spans="1:19" x14ac:dyDescent="0.2">
@@ -9886,7 +9886,7 @@
       </c>
       <c r="S218">
         <f ca="1"/>
-        <v>180</v>
+        <v>222</v>
       </c>
     </row>
     <row r="219" spans="1:19" x14ac:dyDescent="0.2">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="S219">
         <f ca="1"/>
-        <v>24</v>
+        <v>235</v>
       </c>
     </row>
     <row r="220" spans="1:19" x14ac:dyDescent="0.2">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="S220">
         <f ca="1"/>
-        <v>77</v>
+        <v>132</v>
       </c>
     </row>
     <row r="221" spans="1:19" x14ac:dyDescent="0.2">
@@ -10018,7 +10018,7 @@
       </c>
       <c r="S221">
         <f ca="1"/>
-        <v>146</v>
+        <v>41</v>
       </c>
     </row>
     <row r="222" spans="1:19" x14ac:dyDescent="0.2">
@@ -10062,7 +10062,7 @@
       </c>
       <c r="S222">
         <f ca="1"/>
-        <v>152</v>
+        <v>171</v>
       </c>
     </row>
     <row r="223" spans="1:19" x14ac:dyDescent="0.2">
@@ -10106,7 +10106,7 @@
       </c>
       <c r="S223">
         <f ca="1"/>
-        <v>236</v>
+        <v>215</v>
       </c>
     </row>
     <row r="224" spans="1:19" x14ac:dyDescent="0.2">
@@ -10150,7 +10150,7 @@
       </c>
       <c r="S224">
         <f ca="1"/>
-        <v>237</v>
+        <v>43</v>
       </c>
     </row>
     <row r="225" spans="1:19" x14ac:dyDescent="0.2">
@@ -10194,7 +10194,7 @@
       </c>
       <c r="S225">
         <f ca="1"/>
-        <v>206</v>
+        <v>133</v>
       </c>
     </row>
     <row r="226" spans="1:19" x14ac:dyDescent="0.2">
@@ -10230,7 +10230,7 @@
       </c>
       <c r="K226">
         <f t="shared" ca="1" si="7"/>
-        <v>3.2315148430888917E-3</v>
+        <v>0</v>
       </c>
       <c r="N226">
         <f t="shared" si="8"/>
@@ -10238,7 +10238,7 @@
       </c>
       <c r="S226">
         <f ca="1"/>
-        <v>9</v>
+        <v>232</v>
       </c>
     </row>
     <row r="227" spans="1:19" x14ac:dyDescent="0.2">
@@ -10282,7 +10282,7 @@
       </c>
       <c r="S227">
         <f ca="1"/>
-        <v>239</v>
+        <v>192</v>
       </c>
     </row>
     <row r="228" spans="1:19" x14ac:dyDescent="0.2">
@@ -10326,7 +10326,7 @@
       </c>
       <c r="S228">
         <f ca="1"/>
-        <v>57</v>
+        <v>207</v>
       </c>
     </row>
     <row r="229" spans="1:19" x14ac:dyDescent="0.2">
@@ -10362,7 +10362,7 @@
       </c>
       <c r="K229">
         <f t="shared" ca="1" si="7"/>
-        <v>8.4188803944528941E-3</v>
+        <v>0</v>
       </c>
       <c r="N229">
         <f t="shared" si="8"/>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="S229">
         <f ca="1"/>
-        <v>4</v>
+        <v>123</v>
       </c>
     </row>
     <row r="230" spans="1:19" x14ac:dyDescent="0.2">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="S230">
         <f ca="1"/>
-        <v>217</v>
+        <v>121</v>
       </c>
     </row>
     <row r="231" spans="1:19" x14ac:dyDescent="0.2">
@@ -10450,7 +10450,7 @@
       </c>
       <c r="K231">
         <f t="shared" ca="1" si="7"/>
-        <v>3.8530597256941613E-3</v>
+        <v>0</v>
       </c>
       <c r="N231">
         <f t="shared" si="8"/>
@@ -10458,7 +10458,7 @@
       </c>
       <c r="S231">
         <f ca="1"/>
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="232" spans="1:19" x14ac:dyDescent="0.2">
@@ -10502,7 +10502,7 @@
       </c>
       <c r="S232">
         <f ca="1"/>
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="233" spans="1:19" x14ac:dyDescent="0.2">
@@ -10546,7 +10546,7 @@
       </c>
       <c r="S233">
         <f ca="1"/>
-        <v>74</v>
+        <v>205</v>
       </c>
     </row>
     <row r="234" spans="1:19" x14ac:dyDescent="0.2">
@@ -10590,7 +10590,7 @@
       </c>
       <c r="S234">
         <f ca="1"/>
-        <v>187</v>
+        <v>162</v>
       </c>
     </row>
     <row r="235" spans="1:19" x14ac:dyDescent="0.2">
@@ -10634,7 +10634,7 @@
       </c>
       <c r="S235">
         <f ca="1"/>
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="236" spans="1:19" x14ac:dyDescent="0.2">
@@ -10678,7 +10678,7 @@
       </c>
       <c r="S236">
         <f ca="1"/>
-        <v>186</v>
+        <v>238</v>
       </c>
     </row>
     <row r="237" spans="1:19" x14ac:dyDescent="0.2">
@@ -10722,7 +10722,7 @@
       </c>
       <c r="S237">
         <f ca="1"/>
-        <v>216</v>
+        <v>110</v>
       </c>
     </row>
     <row r="238" spans="1:19" x14ac:dyDescent="0.2">
@@ -10766,7 +10766,7 @@
       </c>
       <c r="S238">
         <f ca="1"/>
-        <v>18</v>
+        <v>65</v>
       </c>
     </row>
     <row r="239" spans="1:19" x14ac:dyDescent="0.2">
@@ -10810,7 +10810,7 @@
       </c>
       <c r="S239">
         <f ca="1"/>
-        <v>17</v>
+        <v>185</v>
       </c>
     </row>
     <row r="240" spans="1:19" x14ac:dyDescent="0.2">
@@ -10854,7 +10854,7 @@
       </c>
       <c r="S240">
         <f ca="1"/>
-        <v>12</v>
+        <v>191</v>
       </c>
     </row>
     <row r="241" spans="1:19" x14ac:dyDescent="0.2">
@@ -10898,7 +10898,7 @@
       </c>
       <c r="S241">
         <f ca="1"/>
-        <v>228</v>
+        <v>92</v>
       </c>
     </row>
     <row r="242" spans="1:19" x14ac:dyDescent="0.2">
@@ -10942,7 +10942,7 @@
       </c>
       <c r="S242">
         <f ca="1"/>
-        <v>246</v>
+        <v>45</v>
       </c>
     </row>
     <row r="243" spans="1:19" x14ac:dyDescent="0.2">
@@ -10986,7 +10986,7 @@
       </c>
       <c r="S243">
         <f ca="1"/>
-        <v>122</v>
+        <v>96</v>
       </c>
     </row>
     <row r="244" spans="1:19" x14ac:dyDescent="0.2">
@@ -11030,7 +11030,7 @@
       </c>
       <c r="S244">
         <f ca="1"/>
-        <v>108</v>
+        <v>119</v>
       </c>
     </row>
     <row r="245" spans="1:19" x14ac:dyDescent="0.2">
@@ -11074,7 +11074,7 @@
       </c>
       <c r="S245">
         <f ca="1"/>
-        <v>231</v>
+        <v>120</v>
       </c>
     </row>
     <row r="246" spans="1:19" x14ac:dyDescent="0.2">
@@ -11118,7 +11118,7 @@
       </c>
       <c r="S246">
         <f ca="1"/>
-        <v>214</v>
+        <v>138</v>
       </c>
     </row>
     <row r="247" spans="1:19" x14ac:dyDescent="0.2">
@@ -11162,7 +11162,7 @@
       </c>
       <c r="S247">
         <f ca="1"/>
-        <v>75</v>
+        <v>181</v>
       </c>
     </row>
     <row r="248" spans="1:19" x14ac:dyDescent="0.2">
@@ -11206,7 +11206,7 @@
       </c>
       <c r="S248">
         <f ca="1"/>
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="249" spans="1:19" x14ac:dyDescent="0.2">
@@ -11250,7 +11250,7 @@
       </c>
       <c r="S249">
         <f ca="1"/>
-        <v>67</v>
+        <v>221</v>
       </c>
     </row>
     <row r="250" spans="1:19" x14ac:dyDescent="0.2">
@@ -11294,7 +11294,7 @@
       </c>
       <c r="S250">
         <f ca="1"/>
-        <v>100</v>
+        <v>186</v>
       </c>
     </row>
     <row r="251" spans="1:19" x14ac:dyDescent="0.2">
@@ -11338,7 +11338,7 @@
       </c>
       <c r="S251">
         <f ca="1"/>
-        <v>14</v>
+        <v>216</v>
       </c>
     </row>
     <row r="252" spans="1:19" x14ac:dyDescent="0.2">
@@ -11374,7 +11374,7 @@
       </c>
       <c r="K252">
         <f t="shared" ca="1" si="7"/>
-        <v>1.5505517366166972E-2</v>
+        <v>0</v>
       </c>
       <c r="N252">
         <f t="shared" si="8"/>
@@ -11382,7 +11382,7 @@
       </c>
       <c r="S252">
         <f ca="1"/>
-        <v>10</v>
+        <v>247</v>
       </c>
     </row>
     <row r="253" spans="1:19" x14ac:dyDescent="0.2">
@@ -11426,7 +11426,7 @@
       </c>
       <c r="S253">
         <f ca="1"/>
-        <v>245</v>
+        <v>169</v>
       </c>
     </row>
     <row r="254" spans="1:19" x14ac:dyDescent="0.2">
@@ -11470,7 +11470,7 @@
       </c>
       <c r="S254">
         <f ca="1"/>
-        <v>138</v>
+        <v>242</v>
       </c>
     </row>
     <row r="255" spans="1:19" x14ac:dyDescent="0.2">
@@ -11506,7 +11506,7 @@
       </c>
       <c r="K255">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>4.9654648227392961E-3</v>
       </c>
       <c r="N255">
         <f t="shared" si="8"/>
@@ -11514,7 +11514,7 @@
       </c>
       <c r="S255">
         <f ca="1"/>
-        <v>106</v>
+        <v>5</v>
       </c>
     </row>
     <row r="256" spans="1:19" x14ac:dyDescent="0.2">
@@ -11558,7 +11558,7 @@
       </c>
       <c r="S256">
         <f ca="1"/>
-        <v>87</v>
+        <v>209</v>
       </c>
     </row>
     <row r="257" spans="1:19" x14ac:dyDescent="0.2">
@@ -11602,7 +11602,7 @@
       </c>
       <c r="S257">
         <f ca="1"/>
-        <v>61</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>